<commit_message>
Added reading of outcomeRelations added javadocs renamed main class
</commit_message>
<xml_diff>
--- a/resources/Matrix.xlsx
+++ b/resources/Matrix.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Metz\Dropbox\Studium\Master\Masterarbeit\Arbeitsdateien\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20730" windowHeight="11760" tabRatio="532" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17085" windowHeight="6945" tabRatio="532" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge Base" sheetId="10" r:id="rId1"/>
@@ -21,7 +16,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Knowledge Base'!$B$1:$H$73</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
+  <oleSize ref="A1:T15"/>
 </workbook>
 </file>
 
@@ -31,7 +27,7 @@
     <author>Metz</author>
   </authors>
   <commentList>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN25" authorId="0" shapeId="0">
+    <comment ref="AN25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K31" authorId="0" shapeId="0">
+    <comment ref="K31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K37" authorId="0" shapeId="0">
+    <comment ref="K37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P37" authorId="0" shapeId="0">
+    <comment ref="P37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ49" authorId="0" shapeId="0">
+    <comment ref="AJ49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX49" authorId="0" shapeId="0">
+    <comment ref="AX49" authorId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ51" authorId="0" shapeId="0">
+    <comment ref="AJ51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD54" authorId="0" shapeId="0">
+    <comment ref="AD54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -247,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX54" authorId="0" shapeId="0">
+    <comment ref="AX54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K57" authorId="0" shapeId="0">
+    <comment ref="K57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -295,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T57" authorId="0" shapeId="0">
+    <comment ref="T57" authorId="0">
       <text>
         <r>
           <rPr>
@@ -319,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS76" authorId="0" shapeId="0">
+    <comment ref="AS76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2077,14 +2073,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2107,10 +2103,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2148,133 +2144,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="2" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Null" xfId="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -2348,6 +2222,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2367,9 +2262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2407,9 +2302,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2444,7 +2339,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2479,7 +2374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2705,7 +2600,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="190" t="s">
         <v>159</v>
       </c>
       <c r="B2" s="189" t="s">
@@ -2728,7 +2623,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="188"/>
+      <c r="A3" s="190"/>
       <c r="B3" s="189"/>
       <c r="C3" t="s">
         <v>7</v>
@@ -2741,7 +2636,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="188"/>
+      <c r="A4" s="190"/>
       <c r="B4" s="189"/>
       <c r="C4" t="s">
         <v>115</v>
@@ -2751,35 +2646,35 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="188"/>
+      <c r="A5" s="190"/>
       <c r="B5" s="189"/>
       <c r="C5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="188"/>
+      <c r="A6" s="190"/>
       <c r="B6" s="189"/>
       <c r="C6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="188"/>
+      <c r="A7" s="190"/>
       <c r="B7" s="189"/>
       <c r="C7" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="188"/>
+      <c r="A8" s="190"/>
       <c r="B8" s="189"/>
       <c r="C8" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="188"/>
+      <c r="A9" s="190"/>
       <c r="B9" s="189" t="s">
         <v>124</v>
       </c>
@@ -2794,21 +2689,21 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="188"/>
+      <c r="A10" s="190"/>
       <c r="B10" s="189"/>
       <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="188"/>
+      <c r="A11" s="190"/>
       <c r="B11" s="189"/>
       <c r="C11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="188"/>
+      <c r="A12" s="190"/>
       <c r="B12" s="189"/>
       <c r="C12" t="s">
         <v>120</v>
@@ -2818,7 +2713,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="188"/>
+      <c r="A13" s="190"/>
       <c r="B13" s="189"/>
       <c r="C13" t="s">
         <v>121</v>
@@ -2828,21 +2723,21 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="188"/>
+      <c r="A14" s="190"/>
       <c r="B14" s="189"/>
       <c r="C14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="188"/>
+      <c r="A15" s="190"/>
       <c r="B15" s="189"/>
       <c r="C15" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="188"/>
+      <c r="A16" s="190"/>
       <c r="B16" s="189" t="s">
         <v>125</v>
       </c>
@@ -2860,7 +2755,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="188"/>
+      <c r="A17" s="190"/>
       <c r="B17" s="189"/>
       <c r="C17" t="s">
         <v>4</v>
@@ -2870,7 +2765,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="188"/>
+      <c r="A18" s="190"/>
       <c r="B18" s="189"/>
       <c r="C18" t="s">
         <v>90</v>
@@ -2880,7 +2775,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="188"/>
+      <c r="A19" s="190"/>
       <c r="B19" s="189"/>
       <c r="C19" t="s">
         <v>105</v>
@@ -2893,35 +2788,35 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="188"/>
+      <c r="A20" s="190"/>
       <c r="B20" s="189"/>
       <c r="C20" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="188"/>
+      <c r="A21" s="190"/>
       <c r="B21" s="189"/>
       <c r="C21" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="188"/>
+      <c r="A22" s="190"/>
       <c r="B22" s="189"/>
       <c r="C22" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="188"/>
+      <c r="A23" s="190"/>
       <c r="B23" s="189"/>
       <c r="C23" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="188"/>
+      <c r="A24" s="190"/>
       <c r="B24" s="189" t="s">
         <v>138</v>
       </c>
@@ -2942,7 +2837,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="188"/>
+      <c r="A25" s="190"/>
       <c r="B25" s="189"/>
       <c r="C25" t="s">
         <v>127</v>
@@ -2958,7 +2853,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="188"/>
+      <c r="A26" s="190"/>
       <c r="B26" s="189"/>
       <c r="C26" t="s">
         <v>128</v>
@@ -2974,7 +2869,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="188"/>
+      <c r="A27" s="190"/>
       <c r="B27" s="189"/>
       <c r="C27" t="s">
         <v>129</v>
@@ -2990,7 +2885,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="188" t="s">
+      <c r="A28" s="190" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="189" t="s">
@@ -3010,7 +2905,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="188"/>
+      <c r="A29" s="190"/>
       <c r="B29" s="189"/>
       <c r="C29" t="s">
         <v>73</v>
@@ -3020,42 +2915,42 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="188"/>
+      <c r="A30" s="190"/>
       <c r="B30" s="189"/>
       <c r="C30" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="188"/>
+      <c r="A31" s="190"/>
       <c r="B31" s="189"/>
       <c r="C31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="188"/>
+      <c r="A32" s="190"/>
       <c r="B32" s="189"/>
       <c r="C32" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="188"/>
+      <c r="A33" s="190"/>
       <c r="B33" s="189"/>
       <c r="C33" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="188"/>
+      <c r="A34" s="190"/>
       <c r="B34" s="189"/>
       <c r="C34" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="188"/>
+      <c r="A35" s="190"/>
       <c r="B35" s="189"/>
       <c r="C35" t="s">
         <v>154</v>
@@ -3063,7 +2958,7 @@
       <c r="F35" s="82"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="188"/>
+      <c r="A36" s="190"/>
       <c r="B36" s="189" t="s">
         <v>140</v>
       </c>
@@ -3078,7 +2973,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="188"/>
+      <c r="A37" s="190"/>
       <c r="B37" s="189"/>
       <c r="C37" t="s">
         <v>74</v>
@@ -3088,7 +2983,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="188"/>
+      <c r="A38" s="190"/>
       <c r="B38" s="189"/>
       <c r="C38" s="90" t="s">
         <v>15</v>
@@ -3098,7 +2993,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="188"/>
+      <c r="A39" s="190"/>
       <c r="B39" s="189" t="s">
         <v>141</v>
       </c>
@@ -3113,28 +3008,28 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="188"/>
+      <c r="A40" s="190"/>
       <c r="B40" s="189"/>
       <c r="C40" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="188"/>
+      <c r="A41" s="190"/>
       <c r="B41" s="189"/>
       <c r="C41" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="188"/>
+      <c r="A42" s="190"/>
       <c r="B42" s="189"/>
       <c r="C42" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="188"/>
+      <c r="A43" s="190"/>
       <c r="B43" s="189"/>
       <c r="C43" t="s">
         <v>134</v>
@@ -3144,7 +3039,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="188"/>
+      <c r="A44" s="190"/>
       <c r="B44" s="189" t="s">
         <v>142</v>
       </c>
@@ -3159,7 +3054,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="188"/>
+      <c r="A45" s="190"/>
       <c r="B45" s="189"/>
       <c r="C45" t="s">
         <v>76</v>
@@ -3169,7 +3064,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="188"/>
+      <c r="A46" s="190"/>
       <c r="B46" s="189"/>
       <c r="C46" s="90" t="s">
         <v>77</v>
@@ -3179,7 +3074,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="188" t="s">
+      <c r="A47" s="190" t="s">
         <v>160</v>
       </c>
       <c r="B47" s="189" t="s">
@@ -3197,7 +3092,7 @@
       <c r="F47" t="s">
         <v>78</v>
       </c>
-      <c r="G47" s="190" t="s">
+      <c r="G47" s="188" t="s">
         <v>82</v>
       </c>
       <c r="H47" t="s">
@@ -3205,7 +3100,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="188"/>
+      <c r="A48" s="190"/>
       <c r="B48" s="189"/>
       <c r="C48" t="s">
         <v>156</v>
@@ -3213,13 +3108,13 @@
       <c r="F48" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="190"/>
+      <c r="G48" s="188"/>
       <c r="H48" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="188"/>
+      <c r="A49" s="190"/>
       <c r="B49" s="189"/>
       <c r="C49" t="s">
         <v>157</v>
@@ -3227,13 +3122,13 @@
       <c r="F49" t="s">
         <v>80</v>
       </c>
-      <c r="G49" s="190"/>
+      <c r="G49" s="188"/>
       <c r="H49" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="188"/>
+      <c r="A50" s="190"/>
       <c r="B50" s="189"/>
       <c r="C50" t="s">
         <v>158</v>
@@ -3241,13 +3136,13 @@
       <c r="F50" t="s">
         <v>81</v>
       </c>
-      <c r="G50" s="190"/>
+      <c r="G50" s="188"/>
       <c r="H50" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="188" t="s">
+      <c r="A51" s="190" t="s">
         <v>165</v>
       </c>
       <c r="B51" s="189" t="s">
@@ -3267,7 +3162,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="188"/>
+      <c r="A52" s="190"/>
       <c r="B52" s="189"/>
       <c r="C52" t="s">
         <v>21</v>
@@ -3277,7 +3172,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="188"/>
+      <c r="A53" s="190"/>
       <c r="B53" s="189"/>
       <c r="C53" t="s">
         <v>22</v>
@@ -3287,7 +3182,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="188"/>
+      <c r="A54" s="190"/>
       <c r="B54" s="189"/>
       <c r="C54" s="90" t="s">
         <v>135</v>
@@ -3300,7 +3195,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="188"/>
+      <c r="A55" s="190"/>
       <c r="B55" s="189" t="s">
         <v>145</v>
       </c>
@@ -3315,7 +3210,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="188"/>
+      <c r="A56" s="190"/>
       <c r="B56" s="189"/>
       <c r="C56" t="s">
         <v>83</v>
@@ -3325,35 +3220,35 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="188"/>
+      <c r="A57" s="190"/>
       <c r="B57" s="189"/>
       <c r="C57" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="188"/>
+      <c r="A58" s="190"/>
       <c r="B58" s="189"/>
       <c r="C58" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="188"/>
+      <c r="A59" s="190"/>
       <c r="B59" s="189"/>
       <c r="C59" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="188"/>
+      <c r="A60" s="190"/>
       <c r="B60" s="189"/>
       <c r="C60" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="188"/>
+      <c r="A61" s="190"/>
       <c r="B61" s="189"/>
       <c r="C61" t="s">
         <v>137</v>
@@ -3363,7 +3258,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="188"/>
+      <c r="A62" s="190"/>
       <c r="B62" s="189" t="s">
         <v>146</v>
       </c>
@@ -3378,7 +3273,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="188"/>
+      <c r="A63" s="190"/>
       <c r="B63" s="189"/>
       <c r="C63" t="s">
         <v>107</v>
@@ -3388,7 +3283,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="188"/>
+      <c r="A64" s="190"/>
       <c r="B64" s="189"/>
       <c r="C64" s="90" t="s">
         <v>26</v>
@@ -3398,7 +3293,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="188"/>
+      <c r="A65" s="190"/>
       <c r="B65" s="189" t="s">
         <v>147</v>
       </c>
@@ -3413,7 +3308,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" s="84" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="188"/>
+      <c r="A66" s="190"/>
       <c r="B66" s="189"/>
       <c r="C66" t="s">
         <v>28</v>
@@ -3425,7 +3320,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" s="84" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="188"/>
+      <c r="A67" s="190"/>
       <c r="B67" s="189"/>
       <c r="C67" t="s">
         <v>29</v>
@@ -3437,7 +3332,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="188"/>
+      <c r="A68" s="190"/>
       <c r="B68" s="189"/>
       <c r="C68" t="s">
         <v>161</v>
@@ -3447,7 +3342,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="188"/>
+      <c r="A69" s="190"/>
       <c r="B69" s="189"/>
       <c r="C69" t="s">
         <v>162</v>
@@ -3457,7 +3352,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="188"/>
+      <c r="A70" s="190"/>
       <c r="B70" s="189"/>
       <c r="C70" t="s">
         <v>164</v>
@@ -3467,7 +3362,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="188"/>
+      <c r="A71" s="190"/>
       <c r="B71" s="189"/>
       <c r="C71" t="s">
         <v>163</v>
@@ -3477,7 +3372,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="188"/>
+      <c r="A72" s="190"/>
       <c r="B72" s="86" t="s">
         <v>148</v>
       </c>
@@ -3492,7 +3387,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="188"/>
+      <c r="A73" s="190"/>
       <c r="B73" s="189" t="s">
         <v>150</v>
       </c>
@@ -3507,14 +3402,14 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="188"/>
+      <c r="A74" s="190"/>
       <c r="B74" s="189"/>
       <c r="C74" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="188"/>
+      <c r="A75" s="190"/>
       <c r="B75" s="189"/>
       <c r="C75" t="s">
         <v>99</v>
@@ -3524,7 +3419,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="188"/>
+      <c r="A76" s="190"/>
       <c r="B76" s="189"/>
       <c r="C76" t="s">
         <v>100</v>
@@ -3534,7 +3429,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="188"/>
+      <c r="A77" s="190"/>
       <c r="B77" s="189"/>
       <c r="C77" s="103" t="s">
         <v>101</v>
@@ -3546,7 +3441,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="188"/>
+      <c r="A78" s="190"/>
       <c r="B78" s="189" t="s">
         <v>149</v>
       </c>
@@ -3567,7 +3462,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="188"/>
+      <c r="A79" s="190"/>
       <c r="B79" s="189"/>
       <c r="C79" t="s">
         <v>169</v>
@@ -3585,13 +3480,6 @@
   </sheetData>
   <autoFilter ref="B1:H79"/>
   <mergeCells count="20">
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B55:B61"/>
-    <mergeCell ref="B47:B50"/>
     <mergeCell ref="A2:A27"/>
     <mergeCell ref="A28:A46"/>
     <mergeCell ref="A47:A50"/>
@@ -3605,6 +3493,13 @@
     <mergeCell ref="B65:B71"/>
     <mergeCell ref="B73:B77"/>
     <mergeCell ref="B78:B79"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B61"/>
+    <mergeCell ref="B47:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4631,13 +4526,13 @@
     <mergeCell ref="A7:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:R18">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"Influencing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Affecting"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"Binding"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4653,11 +4548,11 @@
   </sheetPr>
   <dimension ref="A1:BU159"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BJ33" sqref="BJ33"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4924,13 +4819,13 @@
         <v>Select Application Layer</v>
       </c>
       <c r="E2" s="197"/>
-      <c r="F2" s="198"/>
+      <c r="F2" s="199"/>
       <c r="H2" s="197" t="str">
         <f>'Knowledge Base'!$B$9</f>
         <v>Select Application Tier</v>
       </c>
       <c r="I2" s="197"/>
-      <c r="J2" s="198"/>
+      <c r="J2" s="199"/>
       <c r="K2" s="178"/>
       <c r="L2" s="197" t="str">
         <f>'Knowledge Base'!$B$16</f>
@@ -4938,27 +4833,27 @@
       </c>
       <c r="M2" s="197"/>
       <c r="N2" s="197"/>
-      <c r="O2" s="198"/>
+      <c r="O2" s="199"/>
       <c r="Q2" s="197" t="str">
         <f>'Knowledge Base'!$B$24</f>
         <v>Select Migration Type</v>
       </c>
       <c r="R2" s="197"/>
       <c r="S2" s="197"/>
-      <c r="T2" s="198"/>
+      <c r="T2" s="199"/>
       <c r="V2" s="197" t="str">
         <f>'Knowledge Base'!$B$28</f>
         <v>Define Scalability Level</v>
       </c>
       <c r="W2" s="197"/>
       <c r="X2" s="197"/>
-      <c r="Y2" s="198"/>
+      <c r="Y2" s="199"/>
       <c r="AA2" s="197" t="str">
         <f>'Knowledge Base'!$B$36</f>
         <v>Select Scaling Type</v>
       </c>
       <c r="AB2" s="197"/>
-      <c r="AC2" s="198"/>
+      <c r="AC2" s="199"/>
       <c r="AE2" s="197" t="str">
         <f>'Knowledge Base'!$B$39</f>
         <v>Select Elasticity Automation Degree</v>
@@ -4966,33 +4861,33 @@
       <c r="AF2" s="197"/>
       <c r="AG2" s="197"/>
       <c r="AH2" s="197"/>
-      <c r="AI2" s="198"/>
+      <c r="AI2" s="199"/>
       <c r="AK2" s="197" t="str">
         <f>'Knowledge Base'!$B$44</f>
         <v>Select Scaling Trigger</v>
       </c>
       <c r="AL2" s="197"/>
-      <c r="AM2" s="198"/>
+      <c r="AM2" s="199"/>
       <c r="AO2" s="197" t="str">
         <f>'Knowledge Base'!$B$47</f>
         <v>Select Multi-Tenancy Architecture</v>
       </c>
       <c r="AP2" s="197"/>
       <c r="AQ2" s="197"/>
-      <c r="AR2" s="198"/>
+      <c r="AR2" s="199"/>
       <c r="AT2" s="197" t="str">
         <f>'Knowledge Base'!$B$51</f>
         <v>Select Cloud Deployment Model</v>
       </c>
       <c r="AU2" s="197"/>
       <c r="AV2" s="197"/>
-      <c r="AW2" s="198"/>
+      <c r="AW2" s="199"/>
       <c r="AY2" s="197" t="str">
         <f>'Knowledge Base'!$B$55</f>
         <v>Select Cloud Service Model</v>
       </c>
       <c r="AZ2" s="197"/>
-      <c r="BA2" s="198"/>
+      <c r="BA2" s="199"/>
       <c r="BC2" s="197" t="str">
         <f>'Knowledge Base'!$B$62</f>
         <v>Define Cloud Hosting</v>
@@ -5003,7 +4898,7 @@
         <v>Define Roles of Responsibility</v>
       </c>
       <c r="BG2" s="197"/>
-      <c r="BH2" s="198"/>
+      <c r="BH2" s="199"/>
       <c r="BJ2" s="101" t="str">
         <f>'Knowledge Base'!$B$72</f>
         <v>Select Cloud Vendor</v>
@@ -5015,12 +4910,12 @@
       </c>
       <c r="BM2" s="197"/>
       <c r="BN2" s="197"/>
-      <c r="BO2" s="198"/>
+      <c r="BO2" s="199"/>
       <c r="BQ2" s="197" t="str">
         <f>'Knowledge Base'!$B$78</f>
         <v>Define Resource Location</v>
       </c>
-      <c r="BR2" s="198"/>
+      <c r="BR2" s="199"/>
     </row>
     <row r="3" spans="1:73" s="88" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="122"/>
@@ -5797,7 +5692,7 @@
       <c r="BU9" s="83"/>
     </row>
     <row r="10" spans="1:73" s="109" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="199"/>
+      <c r="A10" s="198"/>
       <c r="B10" s="116" t="str">
         <f>'Knowledge Base'!$C$8</f>
         <v>Presentation + Business + Resource Layer</v>
@@ -6519,7 +6414,7 @@
       <c r="BU17" s="83"/>
     </row>
     <row r="18" spans="1:73" s="109" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="199"/>
+      <c r="A18" s="198"/>
       <c r="B18" s="116" t="str">
         <f>'Knowledge Base'!$C$15</f>
         <v>Client + Application + Data Tier</v>
@@ -7581,7 +7476,7 @@
       <c r="BU26" s="83"/>
     </row>
     <row r="27" spans="1:73" s="110" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="199"/>
+      <c r="A27" s="198"/>
       <c r="B27" s="112" t="str">
         <f>'Knowledge Base'!$C$23</f>
         <v>Application + Middleware Components</v>
@@ -8193,7 +8088,7 @@
       <c r="BU31" s="83"/>
     </row>
     <row r="32" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="199"/>
+      <c r="A32" s="198"/>
       <c r="B32" s="112" t="str">
         <f>'Knowledge Base'!$C$27</f>
         <v>Migration Type IV</v>
@@ -9394,7 +9289,7 @@
       <c r="BU40" s="83"/>
     </row>
     <row r="41" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="199"/>
+      <c r="A41" s="198"/>
       <c r="B41" s="112" t="str">
         <f>'Knowledge Base'!$C$35</f>
         <v>OS/VM + Middleware + Application Level Scaling</v>
@@ -9844,7 +9739,7 @@
       <c r="BU44" s="83"/>
     </row>
     <row r="45" spans="1:73" s="111" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="199"/>
+      <c r="A45" s="198"/>
       <c r="B45" s="112" t="str">
         <f>'Knowledge Base'!$C$38</f>
         <v>Hybrid Scaling</v>
@@ -10498,7 +10393,7 @@
       <c r="BU50" s="83"/>
     </row>
     <row r="51" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="199"/>
+      <c r="A51" s="198"/>
       <c r="B51" s="112" t="str">
         <f>'Knowledge Base'!$C$43</f>
         <v>Automatic Third-Party Scaling</v>
@@ -10951,7 +10846,7 @@
       <c r="BU54" s="83"/>
     </row>
     <row r="55" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="199"/>
+      <c r="A55" s="198"/>
       <c r="B55" s="112" t="str">
         <f>'Knowledge Base'!$C$46</f>
         <v>Proactive Trigger</v>
@@ -11550,7 +11445,7 @@
       <c r="BU59" s="83"/>
     </row>
     <row r="60" spans="1:73" s="111" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="199"/>
+      <c r="A60" s="198"/>
       <c r="B60" s="112" t="str">
         <f>'Knowledge Base'!$C$50</f>
         <v>Multi-Tenancy Architecture 3</v>
@@ -12083,7 +11978,7 @@
       <c r="BU64" s="83"/>
     </row>
     <row r="65" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="199"/>
+      <c r="A65" s="198"/>
       <c r="B65" s="112" t="str">
         <f>'Knowledge Base'!$C$54</f>
         <v xml:space="preserve">Hybrid Cloud </v>
@@ -13120,7 +13015,7 @@
       <c r="BU72" s="83"/>
     </row>
     <row r="73" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="199"/>
+      <c r="A73" s="198"/>
       <c r="B73" s="112" t="str">
         <f>'Knowledge Base'!$C$61</f>
         <v>Iaas + PaaS + SaaS</v>
@@ -13575,7 +13470,7 @@
       <c r="BU76" s="83"/>
     </row>
     <row r="77" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="199"/>
+      <c r="A77" s="198"/>
       <c r="B77" s="112" t="str">
         <f>'Knowledge Base'!$C$64</f>
         <v>Hybrid Hosting</v>
@@ -14374,7 +14269,7 @@
       <c r="BU84" s="83"/>
     </row>
     <row r="85" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="199"/>
+      <c r="A85" s="198"/>
       <c r="B85" s="112" t="str">
         <f>'Knowledge Base'!$C$71</f>
         <v>Role Set 1 + 7 + 8</v>
@@ -15140,7 +15035,7 @@
       <c r="BU92" s="83"/>
     </row>
     <row r="93" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="199"/>
+      <c r="A93" s="198"/>
       <c r="B93" s="112" t="str">
         <f>'Knowledge Base'!$C$77</f>
         <v>Combined Pricing Model</v>
@@ -15441,7 +15336,7 @@
       <c r="BU95" s="83"/>
     </row>
     <row r="96" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="199"/>
+      <c r="A96" s="198"/>
       <c r="B96" s="112" t="str">
         <f>'Knowledge Base'!$C$79</f>
         <v>Data Location outside jurisdiction of company</v>
@@ -20128,6 +20023,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="BQ2:BR2"/>
+    <mergeCell ref="BF2:BH2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="AY2:BA2"/>
+    <mergeCell ref="AT2:AW2"/>
+    <mergeCell ref="BL2:BO2"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A53:A55"/>
     <mergeCell ref="A20:A27"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A4:A10"/>
@@ -20140,42 +20053,24 @@
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="BQ2:BR2"/>
-    <mergeCell ref="BF2:BH2"/>
-    <mergeCell ref="BC2:BD2"/>
-    <mergeCell ref="AY2:BA2"/>
-    <mergeCell ref="AT2:AW2"/>
-    <mergeCell ref="BL2:BO2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:BR41 C42:Y42 AA42:BR42 C43:BR47 C48:AW48 AY48:BR48 C49:BR93 C94:AT94 AV94:BC94 BE94:BR94 C95:BR96">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"eb"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="12" operator="beginsWith" text="!">
+    <cfRule type="beginsWith" dxfId="7" priority="12" operator="beginsWith" text="!">
       <formula>LEFT(C3,LEN("!"))="!"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="14" operator="beginsWith" text="?">
+    <cfRule type="beginsWith" dxfId="6" priority="14" operator="beginsWith" text="?">
       <formula>LEFT(C3,LEN("?"))="?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
       <formula>"ex"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
       <formula>"in"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="17" operator="equal">
       <formula>"a"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20192,7 +20087,7 @@
   </sheetPr>
   <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -20757,10 +20652,10 @@
     <mergeCell ref="A7:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:R18">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22139,7 +22034,7 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:U18">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added reading of tasks and their relations changed serialisation with gson to immitate old json file including order and non null values for treewithout outcomes
</commit_message>
<xml_diff>
--- a/resources/Matrix.xlsx
+++ b/resources/Matrix.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Studium\Master\Masterarbeit\Arbeitsdateien\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17085" windowHeight="6945" tabRatio="532" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="20730" windowHeight="11760" tabRatio="532" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge Base" sheetId="10" r:id="rId1"/>
     <sheet name="Decision Level" sheetId="17" r:id="rId2"/>
     <sheet name="Outcome Level" sheetId="21" r:id="rId3"/>
     <sheet name="Required Level" sheetId="24" r:id="rId4"/>
-    <sheet name="Decision Level PreChange" sheetId="23" state="hidden" r:id="rId5"/>
+    <sheet name="Task Level" sheetId="25" r:id="rId5"/>
+    <sheet name="Decision Level PreChange" sheetId="23" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Knowledge Base'!$B$1:$H$73</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
-  <oleSize ref="A1:T15"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -27,7 +32,7 @@
     <author>Metz</author>
   </authors>
   <commentList>
-    <comment ref="K6" authorId="0">
+    <comment ref="K6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN25" authorId="0">
+    <comment ref="AN25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K31" authorId="0">
+    <comment ref="K31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K37" authorId="0">
+    <comment ref="K37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P37" authorId="0">
+    <comment ref="P37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ49" authorId="0">
+    <comment ref="AJ49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX49" authorId="0">
+    <comment ref="AX49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ51" authorId="0">
+    <comment ref="AJ51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD54" authorId="0">
+    <comment ref="AD54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -243,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX54" authorId="0">
+    <comment ref="AX54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -267,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K57" authorId="0">
+    <comment ref="K57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -291,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T57" authorId="0">
+    <comment ref="T57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS76" authorId="0">
+    <comment ref="AS76" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="200">
   <si>
     <t>Decision Point</t>
   </si>
@@ -908,6 +913,42 @@
   </si>
   <si>
     <t>Affecting</t>
+  </si>
+  <si>
+    <t>Workload Profiling</t>
+  </si>
+  <si>
+    <t>Performance Prediction</t>
+  </si>
+  <si>
+    <t>Effort Estimation</t>
+  </si>
+  <si>
+    <t>Cost Analysis</t>
+  </si>
+  <si>
+    <t>Identification of acceptable QoS Levels</t>
+  </si>
+  <si>
+    <t>Compliance Assurance</t>
+  </si>
+  <si>
+    <t>Identification of Security Concerns</t>
+  </si>
+  <si>
+    <t>Workforce Capabilities Identification</t>
+  </si>
+  <si>
+    <t>Vendor Benchmark</t>
+  </si>
+  <si>
+    <t>Application Analysis</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Affected</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1613,7 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2073,6 +2114,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2142,13 +2189,53 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="2" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Null" xfId="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -2160,6 +2247,48 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2225,7 +2354,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2239,7 +2368,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2262,9 +2391,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2302,9 +2431,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2339,7 +2468,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2374,7 +2503,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2600,10 +2729,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="190" t="s">
+      <c r="A2" s="192" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="189" t="s">
+      <c r="B2" s="191" t="s">
         <v>123</v>
       </c>
       <c r="C2" t="s">
@@ -2623,8 +2752,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="190"/>
-      <c r="B3" s="189"/>
+      <c r="A3" s="192"/>
+      <c r="B3" s="191"/>
       <c r="C3" t="s">
         <v>7</v>
       </c>
@@ -2636,8 +2765,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="190"/>
-      <c r="B4" s="189"/>
+      <c r="A4" s="192"/>
+      <c r="B4" s="191"/>
       <c r="C4" t="s">
         <v>115</v>
       </c>
@@ -2646,36 +2775,36 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="190"/>
-      <c r="B5" s="189"/>
+      <c r="A5" s="192"/>
+      <c r="B5" s="191"/>
       <c r="C5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="190"/>
-      <c r="B6" s="189"/>
+      <c r="A6" s="192"/>
+      <c r="B6" s="191"/>
       <c r="C6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="190"/>
-      <c r="B7" s="189"/>
+      <c r="A7" s="192"/>
+      <c r="B7" s="191"/>
       <c r="C7" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="190"/>
-      <c r="B8" s="189"/>
+      <c r="A8" s="192"/>
+      <c r="B8" s="191"/>
       <c r="C8" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="190"/>
-      <c r="B9" s="189" t="s">
+      <c r="A9" s="192"/>
+      <c r="B9" s="191" t="s">
         <v>124</v>
       </c>
       <c r="C9" t="s">
@@ -2689,22 +2818,22 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="190"/>
-      <c r="B10" s="189"/>
+      <c r="A10" s="192"/>
+      <c r="B10" s="191"/>
       <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="190"/>
-      <c r="B11" s="189"/>
+      <c r="A11" s="192"/>
+      <c r="B11" s="191"/>
       <c r="C11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="190"/>
-      <c r="B12" s="189"/>
+      <c r="A12" s="192"/>
+      <c r="B12" s="191"/>
       <c r="C12" t="s">
         <v>120</v>
       </c>
@@ -2713,8 +2842,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="190"/>
-      <c r="B13" s="189"/>
+      <c r="A13" s="192"/>
+      <c r="B13" s="191"/>
       <c r="C13" t="s">
         <v>121</v>
       </c>
@@ -2723,22 +2852,22 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="190"/>
-      <c r="B14" s="189"/>
+      <c r="A14" s="192"/>
+      <c r="B14" s="191"/>
       <c r="C14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="190"/>
-      <c r="B15" s="189"/>
+      <c r="A15" s="192"/>
+      <c r="B15" s="191"/>
       <c r="C15" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="190"/>
-      <c r="B16" s="189" t="s">
+      <c r="A16" s="192"/>
+      <c r="B16" s="191" t="s">
         <v>125</v>
       </c>
       <c r="C16" t="s">
@@ -2755,8 +2884,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="190"/>
-      <c r="B17" s="189"/>
+      <c r="A17" s="192"/>
+      <c r="B17" s="191"/>
       <c r="C17" t="s">
         <v>4</v>
       </c>
@@ -2765,8 +2894,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="190"/>
-      <c r="B18" s="189"/>
+      <c r="A18" s="192"/>
+      <c r="B18" s="191"/>
       <c r="C18" t="s">
         <v>90</v>
       </c>
@@ -2775,8 +2904,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="190"/>
-      <c r="B19" s="189"/>
+      <c r="A19" s="192"/>
+      <c r="B19" s="191"/>
       <c r="C19" t="s">
         <v>105</v>
       </c>
@@ -2788,36 +2917,36 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="190"/>
-      <c r="B20" s="189"/>
+      <c r="A20" s="192"/>
+      <c r="B20" s="191"/>
       <c r="C20" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="190"/>
-      <c r="B21" s="189"/>
+      <c r="A21" s="192"/>
+      <c r="B21" s="191"/>
       <c r="C21" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="190"/>
-      <c r="B22" s="189"/>
+      <c r="A22" s="192"/>
+      <c r="B22" s="191"/>
       <c r="C22" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="190"/>
-      <c r="B23" s="189"/>
+      <c r="A23" s="192"/>
+      <c r="B23" s="191"/>
       <c r="C23" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="190"/>
-      <c r="B24" s="189" t="s">
+      <c r="A24" s="192"/>
+      <c r="B24" s="191" t="s">
         <v>138</v>
       </c>
       <c r="C24" t="s">
@@ -2837,8 +2966,8 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="190"/>
-      <c r="B25" s="189"/>
+      <c r="A25" s="192"/>
+      <c r="B25" s="191"/>
       <c r="C25" t="s">
         <v>127</v>
       </c>
@@ -2853,8 +2982,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="190"/>
-      <c r="B26" s="189"/>
+      <c r="A26" s="192"/>
+      <c r="B26" s="191"/>
       <c r="C26" t="s">
         <v>128</v>
       </c>
@@ -2869,8 +2998,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="190"/>
-      <c r="B27" s="189"/>
+      <c r="A27" s="192"/>
+      <c r="B27" s="191"/>
       <c r="C27" t="s">
         <v>129</v>
       </c>
@@ -2885,10 +3014,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="190" t="s">
+      <c r="A28" s="192" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="189" t="s">
+      <c r="B28" s="191" t="s">
         <v>139</v>
       </c>
       <c r="C28" s="82" t="s">
@@ -2905,8 +3034,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="190"/>
-      <c r="B29" s="189"/>
+      <c r="A29" s="192"/>
+      <c r="B29" s="191"/>
       <c r="C29" t="s">
         <v>73</v>
       </c>
@@ -2915,51 +3044,51 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="190"/>
-      <c r="B30" s="189"/>
+      <c r="A30" s="192"/>
+      <c r="B30" s="191"/>
       <c r="C30" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="190"/>
-      <c r="B31" s="189"/>
+      <c r="A31" s="192"/>
+      <c r="B31" s="191"/>
       <c r="C31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="190"/>
-      <c r="B32" s="189"/>
+      <c r="A32" s="192"/>
+      <c r="B32" s="191"/>
       <c r="C32" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="190"/>
-      <c r="B33" s="189"/>
+      <c r="A33" s="192"/>
+      <c r="B33" s="191"/>
       <c r="C33" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="190"/>
-      <c r="B34" s="189"/>
+      <c r="A34" s="192"/>
+      <c r="B34" s="191"/>
       <c r="C34" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="190"/>
-      <c r="B35" s="189"/>
+      <c r="A35" s="192"/>
+      <c r="B35" s="191"/>
       <c r="C35" t="s">
         <v>154</v>
       </c>
       <c r="F35" s="82"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="190"/>
-      <c r="B36" s="189" t="s">
+      <c r="A36" s="192"/>
+      <c r="B36" s="191" t="s">
         <v>140</v>
       </c>
       <c r="C36" t="s">
@@ -2973,8 +3102,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="190"/>
-      <c r="B37" s="189"/>
+      <c r="A37" s="192"/>
+      <c r="B37" s="191"/>
       <c r="C37" t="s">
         <v>74</v>
       </c>
@@ -2983,8 +3112,8 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="190"/>
-      <c r="B38" s="189"/>
+      <c r="A38" s="192"/>
+      <c r="B38" s="191"/>
       <c r="C38" s="90" t="s">
         <v>15</v>
       </c>
@@ -2993,8 +3122,8 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="190"/>
-      <c r="B39" s="189" t="s">
+      <c r="A39" s="192"/>
+      <c r="B39" s="191" t="s">
         <v>141</v>
       </c>
       <c r="C39" t="s">
@@ -3008,29 +3137,29 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="190"/>
-      <c r="B40" s="189"/>
+      <c r="A40" s="192"/>
+      <c r="B40" s="191"/>
       <c r="C40" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="190"/>
-      <c r="B41" s="189"/>
+      <c r="A41" s="192"/>
+      <c r="B41" s="191"/>
       <c r="C41" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="190"/>
-      <c r="B42" s="189"/>
+      <c r="A42" s="192"/>
+      <c r="B42" s="191"/>
       <c r="C42" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="190"/>
-      <c r="B43" s="189"/>
+      <c r="A43" s="192"/>
+      <c r="B43" s="191"/>
       <c r="C43" t="s">
         <v>134</v>
       </c>
@@ -3039,8 +3168,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="190"/>
-      <c r="B44" s="189" t="s">
+      <c r="A44" s="192"/>
+      <c r="B44" s="191" t="s">
         <v>142</v>
       </c>
       <c r="C44" t="s">
@@ -3054,8 +3183,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="190"/>
-      <c r="B45" s="189"/>
+      <c r="A45" s="192"/>
+      <c r="B45" s="191"/>
       <c r="C45" t="s">
         <v>76</v>
       </c>
@@ -3064,8 +3193,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="190"/>
-      <c r="B46" s="189"/>
+      <c r="A46" s="192"/>
+      <c r="B46" s="191"/>
       <c r="C46" s="90" t="s">
         <v>77</v>
       </c>
@@ -3074,10 +3203,10 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="190" t="s">
+      <c r="A47" s="192" t="s">
         <v>160</v>
       </c>
-      <c r="B47" s="189" t="s">
+      <c r="B47" s="191" t="s">
         <v>143</v>
       </c>
       <c r="C47" t="s">
@@ -3092,7 +3221,7 @@
       <c r="F47" t="s">
         <v>78</v>
       </c>
-      <c r="G47" s="188" t="s">
+      <c r="G47" s="190" t="s">
         <v>82</v>
       </c>
       <c r="H47" t="s">
@@ -3100,52 +3229,52 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="190"/>
-      <c r="B48" s="189"/>
+      <c r="A48" s="192"/>
+      <c r="B48" s="191"/>
       <c r="C48" t="s">
         <v>156</v>
       </c>
       <c r="F48" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="188"/>
+      <c r="G48" s="190"/>
       <c r="H48" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="190"/>
-      <c r="B49" s="189"/>
+      <c r="A49" s="192"/>
+      <c r="B49" s="191"/>
       <c r="C49" t="s">
         <v>157</v>
       </c>
       <c r="F49" t="s">
         <v>80</v>
       </c>
-      <c r="G49" s="188"/>
+      <c r="G49" s="190"/>
       <c r="H49" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="190"/>
-      <c r="B50" s="189"/>
+      <c r="A50" s="192"/>
+      <c r="B50" s="191"/>
       <c r="C50" t="s">
         <v>158</v>
       </c>
       <c r="F50" t="s">
         <v>81</v>
       </c>
-      <c r="G50" s="188"/>
+      <c r="G50" s="190"/>
       <c r="H50" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="190" t="s">
+      <c r="A51" s="192" t="s">
         <v>165</v>
       </c>
-      <c r="B51" s="189" t="s">
+      <c r="B51" s="191" t="s">
         <v>144</v>
       </c>
       <c r="C51" t="s">
@@ -3162,8 +3291,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="190"/>
-      <c r="B52" s="189"/>
+      <c r="A52" s="192"/>
+      <c r="B52" s="191"/>
       <c r="C52" t="s">
         <v>21</v>
       </c>
@@ -3172,8 +3301,8 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="190"/>
-      <c r="B53" s="189"/>
+      <c r="A53" s="192"/>
+      <c r="B53" s="191"/>
       <c r="C53" t="s">
         <v>22</v>
       </c>
@@ -3182,8 +3311,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="190"/>
-      <c r="B54" s="189"/>
+      <c r="A54" s="192"/>
+      <c r="B54" s="191"/>
       <c r="C54" s="90" t="s">
         <v>135</v>
       </c>
@@ -3195,8 +3324,8 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="190"/>
-      <c r="B55" s="189" t="s">
+      <c r="A55" s="192"/>
+      <c r="B55" s="191" t="s">
         <v>145</v>
       </c>
       <c r="C55" t="s">
@@ -3210,8 +3339,8 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="190"/>
-      <c r="B56" s="189"/>
+      <c r="A56" s="192"/>
+      <c r="B56" s="191"/>
       <c r="C56" t="s">
         <v>83</v>
       </c>
@@ -3220,36 +3349,36 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="190"/>
-      <c r="B57" s="189"/>
+      <c r="A57" s="192"/>
+      <c r="B57" s="191"/>
       <c r="C57" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="190"/>
-      <c r="B58" s="189"/>
+      <c r="A58" s="192"/>
+      <c r="B58" s="191"/>
       <c r="C58" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="190"/>
-      <c r="B59" s="189"/>
+      <c r="A59" s="192"/>
+      <c r="B59" s="191"/>
       <c r="C59" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="190"/>
-      <c r="B60" s="189"/>
+      <c r="A60" s="192"/>
+      <c r="B60" s="191"/>
       <c r="C60" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="190"/>
-      <c r="B61" s="189"/>
+      <c r="A61" s="192"/>
+      <c r="B61" s="191"/>
       <c r="C61" t="s">
         <v>137</v>
       </c>
@@ -3258,8 +3387,8 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="190"/>
-      <c r="B62" s="189" t="s">
+      <c r="A62" s="192"/>
+      <c r="B62" s="191" t="s">
         <v>146</v>
       </c>
       <c r="C62" t="s">
@@ -3273,8 +3402,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="190"/>
-      <c r="B63" s="189"/>
+      <c r="A63" s="192"/>
+      <c r="B63" s="191"/>
       <c r="C63" t="s">
         <v>107</v>
       </c>
@@ -3283,8 +3412,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="190"/>
-      <c r="B64" s="189"/>
+      <c r="A64" s="192"/>
+      <c r="B64" s="191"/>
       <c r="C64" s="90" t="s">
         <v>26</v>
       </c>
@@ -3293,8 +3422,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="190"/>
-      <c r="B65" s="189" t="s">
+      <c r="A65" s="192"/>
+      <c r="B65" s="191" t="s">
         <v>147</v>
       </c>
       <c r="C65" t="s">
@@ -3308,8 +3437,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" s="84" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="190"/>
-      <c r="B66" s="189"/>
+      <c r="A66" s="192"/>
+      <c r="B66" s="191"/>
       <c r="C66" t="s">
         <v>28</v>
       </c>
@@ -3320,8 +3449,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" s="84" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="190"/>
-      <c r="B67" s="189"/>
+      <c r="A67" s="192"/>
+      <c r="B67" s="191"/>
       <c r="C67" t="s">
         <v>29</v>
       </c>
@@ -3332,8 +3461,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="190"/>
-      <c r="B68" s="189"/>
+      <c r="A68" s="192"/>
+      <c r="B68" s="191"/>
       <c r="C68" t="s">
         <v>161</v>
       </c>
@@ -3342,8 +3471,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="190"/>
-      <c r="B69" s="189"/>
+      <c r="A69" s="192"/>
+      <c r="B69" s="191"/>
       <c r="C69" t="s">
         <v>162</v>
       </c>
@@ -3352,8 +3481,8 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="190"/>
-      <c r="B70" s="189"/>
+      <c r="A70" s="192"/>
+      <c r="B70" s="191"/>
       <c r="C70" t="s">
         <v>164</v>
       </c>
@@ -3362,8 +3491,8 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="190"/>
-      <c r="B71" s="189"/>
+      <c r="A71" s="192"/>
+      <c r="B71" s="191"/>
       <c r="C71" t="s">
         <v>163</v>
       </c>
@@ -3372,7 +3501,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="190"/>
+      <c r="A72" s="192"/>
       <c r="B72" s="86" t="s">
         <v>148</v>
       </c>
@@ -3387,8 +3516,8 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="190"/>
-      <c r="B73" s="189" t="s">
+      <c r="A73" s="192"/>
+      <c r="B73" s="191" t="s">
         <v>150</v>
       </c>
       <c r="C73" t="s">
@@ -3402,15 +3531,15 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="190"/>
-      <c r="B74" s="189"/>
+      <c r="A74" s="192"/>
+      <c r="B74" s="191"/>
       <c r="C74" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="190"/>
-      <c r="B75" s="189"/>
+      <c r="A75" s="192"/>
+      <c r="B75" s="191"/>
       <c r="C75" t="s">
         <v>99</v>
       </c>
@@ -3419,8 +3548,8 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="190"/>
-      <c r="B76" s="189"/>
+      <c r="A76" s="192"/>
+      <c r="B76" s="191"/>
       <c r="C76" t="s">
         <v>100</v>
       </c>
@@ -3429,8 +3558,8 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="190"/>
-      <c r="B77" s="189"/>
+      <c r="A77" s="192"/>
+      <c r="B77" s="191"/>
       <c r="C77" s="103" t="s">
         <v>101</v>
       </c>
@@ -3441,8 +3570,8 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="190"/>
-      <c r="B78" s="189" t="s">
+      <c r="A78" s="192"/>
+      <c r="B78" s="191" t="s">
         <v>149</v>
       </c>
       <c r="C78" t="s">
@@ -3462,8 +3591,8 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="190"/>
-      <c r="B79" s="189"/>
+      <c r="A79" s="192"/>
+      <c r="B79" s="191"/>
       <c r="C79" t="s">
         <v>169</v>
       </c>
@@ -3533,34 +3662,34 @@
     <row r="1" spans="1:18" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="127"/>
       <c r="B1" s="128"/>
-      <c r="C1" s="193" t="str">
+      <c r="C1" s="195" t="str">
         <f>'Knowledge Base'!$A$2</f>
         <v>Distribute Application</v>
       </c>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="195" t="str">
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="197" t="str">
         <f>'Knowledge Base'!$A$28</f>
         <v>Define Elasticity Strategy</v>
       </c>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="194"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="196"/>
       <c r="K1" s="123" t="str">
         <f>'Knowledge Base'!$A$47</f>
         <v>Define Multi-Tenancy Requirements</v>
       </c>
-      <c r="L1" s="193" t="str">
+      <c r="L1" s="195" t="str">
         <f>'Knowledge Base'!$A$51</f>
         <v>Select Service Provider / Offering</v>
       </c>
-      <c r="M1" s="193"/>
-      <c r="N1" s="193"/>
-      <c r="O1" s="193"/>
-      <c r="P1" s="193"/>
-      <c r="Q1" s="193"/>
-      <c r="R1" s="194"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+      <c r="O1" s="195"/>
+      <c r="P1" s="195"/>
+      <c r="Q1" s="195"/>
+      <c r="R1" s="196"/>
     </row>
     <row r="2" spans="1:18" s="184" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="127"/>
@@ -3633,7 +3762,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="191" t="str">
+      <c r="A3" s="193" t="str">
         <f>'Knowledge Base'!$A$2</f>
         <v>Distribute Application</v>
       </c>
@@ -3689,7 +3818,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="191"/>
+      <c r="A4" s="193"/>
       <c r="B4" s="130" t="str">
         <f>'Knowledge Base'!$B$9</f>
         <v>Select Application Tier</v>
@@ -3742,7 +3871,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="191"/>
+      <c r="A5" s="193"/>
       <c r="B5" s="130" t="str">
         <f>'Knowledge Base'!$B$16</f>
         <v>Select Application Components</v>
@@ -3795,7 +3924,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="192"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="131" t="str">
         <f>'Knowledge Base'!$B$24</f>
         <v>Select Migration Type</v>
@@ -3848,7 +3977,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="196" t="str">
+      <c r="A7" s="198" t="str">
         <f>'Knowledge Base'!$A$28</f>
         <v>Define Elasticity Strategy</v>
       </c>
@@ -3904,7 +4033,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="191"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="95" t="str">
         <f>'Knowledge Base'!$B$36</f>
         <v>Select Scaling Type</v>
@@ -3957,7 +4086,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="191"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="95" t="str">
         <f>'Knowledge Base'!$B$39</f>
         <v>Select Elasticity Automation Degree</v>
@@ -4010,7 +4139,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="192"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="96" t="str">
         <f>'Knowledge Base'!$B$44</f>
         <v>Select Scaling Trigger</v>
@@ -4119,7 +4248,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="191" t="str">
+      <c r="A12" s="193" t="str">
         <f>'Knowledge Base'!$A$51</f>
         <v>Select Service Provider / Offering</v>
       </c>
@@ -4175,7 +4304,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="191"/>
+      <c r="A13" s="193"/>
       <c r="B13" s="95" t="str">
         <f>'Knowledge Base'!$B$55</f>
         <v>Select Cloud Service Model</v>
@@ -4228,7 +4357,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="191"/>
+      <c r="A14" s="193"/>
       <c r="B14" s="95" t="str">
         <f>'Knowledge Base'!$B$62</f>
         <v>Define Cloud Hosting</v>
@@ -4281,7 +4410,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="191"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="95" t="str">
         <f>'Knowledge Base'!$B$65</f>
         <v>Define Roles of Responsibility</v>
@@ -4334,7 +4463,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="191"/>
+      <c r="A16" s="193"/>
       <c r="B16" s="95" t="str">
         <f>'Knowledge Base'!$B$72</f>
         <v>Select Cloud Vendor</v>
@@ -4387,7 +4516,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="191"/>
+      <c r="A17" s="193"/>
       <c r="B17" s="95" t="str">
         <f>'Knowledge Base'!$B$73</f>
         <v>Select Pricing Model</v>
@@ -4440,7 +4569,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="192"/>
+      <c r="A18" s="194"/>
       <c r="B18" s="174" t="str">
         <f>'Knowledge Base'!$B$78</f>
         <v>Define Resource Location</v>
@@ -4526,14 +4655,14 @@
     <mergeCell ref="A7:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:R18">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
-      <formula>"Influencing"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"Binding"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"Affecting"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"Binding"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+      <formula>"Influencing"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4548,11 +4677,11 @@
   </sheetPr>
   <dimension ref="A1:BU159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4814,108 +4943,108 @@
         <v>1</v>
       </c>
       <c r="B2" s="114"/>
-      <c r="D2" s="197" t="str">
+      <c r="D2" s="199" t="str">
         <f>'Knowledge Base'!$B$2</f>
         <v>Select Application Layer</v>
       </c>
-      <c r="E2" s="197"/>
-      <c r="F2" s="199"/>
-      <c r="H2" s="197" t="str">
+      <c r="E2" s="199"/>
+      <c r="F2" s="201"/>
+      <c r="H2" s="199" t="str">
         <f>'Knowledge Base'!$B$9</f>
         <v>Select Application Tier</v>
       </c>
-      <c r="I2" s="197"/>
-      <c r="J2" s="199"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="201"/>
       <c r="K2" s="178"/>
-      <c r="L2" s="197" t="str">
+      <c r="L2" s="199" t="str">
         <f>'Knowledge Base'!$B$16</f>
         <v>Select Application Components</v>
       </c>
-      <c r="M2" s="197"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="199"/>
-      <c r="Q2" s="197" t="str">
+      <c r="M2" s="199"/>
+      <c r="N2" s="199"/>
+      <c r="O2" s="201"/>
+      <c r="Q2" s="199" t="str">
         <f>'Knowledge Base'!$B$24</f>
         <v>Select Migration Type</v>
       </c>
-      <c r="R2" s="197"/>
-      <c r="S2" s="197"/>
-      <c r="T2" s="199"/>
-      <c r="V2" s="197" t="str">
+      <c r="R2" s="199"/>
+      <c r="S2" s="199"/>
+      <c r="T2" s="201"/>
+      <c r="V2" s="199" t="str">
         <f>'Knowledge Base'!$B$28</f>
         <v>Define Scalability Level</v>
       </c>
-      <c r="W2" s="197"/>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="199"/>
-      <c r="AA2" s="197" t="str">
+      <c r="W2" s="199"/>
+      <c r="X2" s="199"/>
+      <c r="Y2" s="201"/>
+      <c r="AA2" s="199" t="str">
         <f>'Knowledge Base'!$B$36</f>
         <v>Select Scaling Type</v>
       </c>
-      <c r="AB2" s="197"/>
-      <c r="AC2" s="199"/>
-      <c r="AE2" s="197" t="str">
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="201"/>
+      <c r="AE2" s="199" t="str">
         <f>'Knowledge Base'!$B$39</f>
         <v>Select Elasticity Automation Degree</v>
       </c>
-      <c r="AF2" s="197"/>
-      <c r="AG2" s="197"/>
-      <c r="AH2" s="197"/>
-      <c r="AI2" s="199"/>
-      <c r="AK2" s="197" t="str">
+      <c r="AF2" s="199"/>
+      <c r="AG2" s="199"/>
+      <c r="AH2" s="199"/>
+      <c r="AI2" s="201"/>
+      <c r="AK2" s="199" t="str">
         <f>'Knowledge Base'!$B$44</f>
         <v>Select Scaling Trigger</v>
       </c>
-      <c r="AL2" s="197"/>
-      <c r="AM2" s="199"/>
-      <c r="AO2" s="197" t="str">
+      <c r="AL2" s="199"/>
+      <c r="AM2" s="201"/>
+      <c r="AO2" s="199" t="str">
         <f>'Knowledge Base'!$B$47</f>
         <v>Select Multi-Tenancy Architecture</v>
       </c>
-      <c r="AP2" s="197"/>
-      <c r="AQ2" s="197"/>
-      <c r="AR2" s="199"/>
-      <c r="AT2" s="197" t="str">
+      <c r="AP2" s="199"/>
+      <c r="AQ2" s="199"/>
+      <c r="AR2" s="201"/>
+      <c r="AT2" s="199" t="str">
         <f>'Knowledge Base'!$B$51</f>
         <v>Select Cloud Deployment Model</v>
       </c>
-      <c r="AU2" s="197"/>
-      <c r="AV2" s="197"/>
-      <c r="AW2" s="199"/>
-      <c r="AY2" s="197" t="str">
+      <c r="AU2" s="199"/>
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="201"/>
+      <c r="AY2" s="199" t="str">
         <f>'Knowledge Base'!$B$55</f>
         <v>Select Cloud Service Model</v>
       </c>
-      <c r="AZ2" s="197"/>
-      <c r="BA2" s="199"/>
-      <c r="BC2" s="197" t="str">
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="201"/>
+      <c r="BC2" s="199" t="str">
         <f>'Knowledge Base'!$B$62</f>
         <v>Define Cloud Hosting</v>
       </c>
-      <c r="BD2" s="197"/>
-      <c r="BF2" s="197" t="str">
+      <c r="BD2" s="199"/>
+      <c r="BF2" s="199" t="str">
         <f>'Knowledge Base'!$B$65</f>
         <v>Define Roles of Responsibility</v>
       </c>
-      <c r="BG2" s="197"/>
-      <c r="BH2" s="199"/>
+      <c r="BG2" s="199"/>
+      <c r="BH2" s="201"/>
       <c r="BJ2" s="101" t="str">
         <f>'Knowledge Base'!$B$72</f>
         <v>Select Cloud Vendor</v>
       </c>
       <c r="BK2" s="134"/>
-      <c r="BL2" s="197" t="str">
+      <c r="BL2" s="199" t="str">
         <f>'Knowledge Base'!$B$73</f>
         <v>Select Pricing Model</v>
       </c>
-      <c r="BM2" s="197"/>
-      <c r="BN2" s="197"/>
-      <c r="BO2" s="199"/>
-      <c r="BQ2" s="197" t="str">
+      <c r="BM2" s="199"/>
+      <c r="BN2" s="199"/>
+      <c r="BO2" s="201"/>
+      <c r="BQ2" s="199" t="str">
         <f>'Knowledge Base'!$B$78</f>
         <v>Define Resource Location</v>
       </c>
-      <c r="BR2" s="199"/>
+      <c r="BR2" s="201"/>
     </row>
     <row r="3" spans="1:73" s="88" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="122"/>
@@ -5037,7 +5166,7 @@
       <c r="BR3" s="98"/>
     </row>
     <row r="4" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="197" t="str">
+      <c r="A4" s="199" t="str">
         <f>'Knowledge Base'!$B$2</f>
         <v>Select Application Layer</v>
       </c>
@@ -5148,7 +5277,7 @@
       <c r="BU4" s="83"/>
     </row>
     <row r="5" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="197"/>
+      <c r="A5" s="199"/>
       <c r="B5" s="113" t="str">
         <f>'Knowledge Base'!$C$3</f>
         <v>Business Layer</v>
@@ -5258,7 +5387,7 @@
       <c r="BU5" s="83"/>
     </row>
     <row r="6" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="197"/>
+      <c r="A6" s="199"/>
       <c r="B6" s="113" t="str">
         <f>'Knowledge Base'!$C$4</f>
         <v>Resource Layer</v>
@@ -5368,7 +5497,7 @@
       <c r="BU6" s="83"/>
     </row>
     <row r="7" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="197"/>
+      <c r="A7" s="199"/>
       <c r="B7" s="113" t="str">
         <f>'Knowledge Base'!$C$5</f>
         <v>Presentation + Business Layer</v>
@@ -5476,7 +5605,7 @@
       <c r="BU7" s="83"/>
     </row>
     <row r="8" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="197"/>
+      <c r="A8" s="199"/>
       <c r="B8" s="113" t="str">
         <f>'Knowledge Base'!$C$6</f>
         <v>Presentation + Resource Layer</v>
@@ -5584,7 +5713,7 @@
       <c r="BU8" s="83"/>
     </row>
     <row r="9" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="197"/>
+      <c r="A9" s="199"/>
       <c r="B9" s="113" t="str">
         <f>'Knowledge Base'!$C$7</f>
         <v>Business + Resource Layer</v>
@@ -5692,7 +5821,7 @@
       <c r="BU9" s="83"/>
     </row>
     <row r="10" spans="1:73" s="109" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="198"/>
+      <c r="A10" s="200"/>
       <c r="B10" s="116" t="str">
         <f>'Knowledge Base'!$C$8</f>
         <v>Presentation + Business + Resource Layer</v>
@@ -5919,7 +6048,7 @@
       <c r="BR11" s="98"/>
     </row>
     <row r="12" spans="1:73" s="83" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="197" t="str">
+      <c r="A12" s="199" t="str">
         <f>'Knowledge Base'!$B$9</f>
         <v>Select Application Tier</v>
       </c>
@@ -6003,7 +6132,7 @@
       <c r="BR12" s="98"/>
     </row>
     <row r="13" spans="1:73" s="83" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="197"/>
+      <c r="A13" s="199"/>
       <c r="B13" s="115" t="str">
         <f>'Knowledge Base'!$C$10</f>
         <v>Application Tier</v>
@@ -6084,7 +6213,7 @@
       <c r="BR13" s="98"/>
     </row>
     <row r="14" spans="1:73" s="83" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="197"/>
+      <c r="A14" s="199"/>
       <c r="B14" s="115" t="str">
         <f>'Knowledge Base'!$C$11</f>
         <v>Data Tier</v>
@@ -6165,7 +6294,7 @@
       <c r="BR14" s="98"/>
     </row>
     <row r="15" spans="1:73" s="83" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="197"/>
+      <c r="A15" s="199"/>
       <c r="B15" s="115" t="str">
         <f>'Knowledge Base'!$C$12</f>
         <v>Client + Application Tier</v>
@@ -6246,7 +6375,7 @@
       <c r="BR15" s="98"/>
     </row>
     <row r="16" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="197"/>
+      <c r="A16" s="199"/>
       <c r="B16" s="113" t="str">
         <f>'Knowledge Base'!$C$13</f>
         <v>Client + Data Tier</v>
@@ -6330,7 +6459,7 @@
       <c r="BU16" s="83"/>
     </row>
     <row r="17" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="197"/>
+      <c r="A17" s="199"/>
       <c r="B17" s="113" t="str">
         <f>'Knowledge Base'!$C$14</f>
         <v>Application + Data Tier</v>
@@ -6414,7 +6543,7 @@
       <c r="BU17" s="83"/>
     </row>
     <row r="18" spans="1:73" s="109" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="198"/>
+      <c r="A18" s="200"/>
       <c r="B18" s="116" t="str">
         <f>'Knowledge Base'!$C$15</f>
         <v>Client + Application + Data Tier</v>
@@ -6617,7 +6746,7 @@
       <c r="BR19" s="98"/>
     </row>
     <row r="20" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="197" t="str">
+      <c r="A20" s="199" t="str">
         <f>'Knowledge Base'!$B$16</f>
         <v>Select Application Components</v>
       </c>
@@ -6742,7 +6871,7 @@
       <c r="BU20" s="83"/>
     </row>
     <row r="21" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="197"/>
+      <c r="A21" s="199"/>
       <c r="B21" s="113" t="str">
         <f>'Knowledge Base'!$C$17</f>
         <v>Application Components</v>
@@ -6864,7 +6993,7 @@
       <c r="BU21" s="83"/>
     </row>
     <row r="22" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="197"/>
+      <c r="A22" s="199"/>
       <c r="B22" s="113" t="str">
         <f>'Knowledge Base'!$C$18</f>
         <v>Middleware Component</v>
@@ -6986,7 +7115,7 @@
       <c r="BU22" s="83"/>
     </row>
     <row r="23" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="197"/>
+      <c r="A23" s="199"/>
       <c r="B23" s="113" t="str">
         <f>'Knowledge Base'!$C$19</f>
         <v>Middleware Components</v>
@@ -7108,7 +7237,7 @@
       <c r="BU23" s="83"/>
     </row>
     <row r="24" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="197"/>
+      <c r="A24" s="199"/>
       <c r="B24" s="113" t="str">
         <f>'Knowledge Base'!$C$20</f>
         <v>Application + Middleware Component</v>
@@ -7230,7 +7359,7 @@
       <c r="BU24" s="83"/>
     </row>
     <row r="25" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="197"/>
+      <c r="A25" s="199"/>
       <c r="B25" s="113" t="str">
         <f>'Knowledge Base'!$C$21</f>
         <v>Application Component + Middleware Components</v>
@@ -7354,7 +7483,7 @@
       <c r="BU25" s="83"/>
     </row>
     <row r="26" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="197"/>
+      <c r="A26" s="199"/>
       <c r="B26" s="113" t="str">
         <f>'Knowledge Base'!$C$22</f>
         <v>Middleware Component + Application Components</v>
@@ -7476,7 +7605,7 @@
       <c r="BU26" s="83"/>
     </row>
     <row r="27" spans="1:73" s="110" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="198"/>
+      <c r="A27" s="200"/>
       <c r="B27" s="112" t="str">
         <f>'Knowledge Base'!$C$23</f>
         <v>Application + Middleware Components</v>
@@ -7717,7 +7846,7 @@
       <c r="BR28" s="98"/>
     </row>
     <row r="29" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="197" t="str">
+      <c r="A29" s="199" t="str">
         <f>'Knowledge Base'!$B$24</f>
         <v>Select Migration Type</v>
       </c>
@@ -7842,7 +7971,7 @@
       <c r="BU29" s="83"/>
     </row>
     <row r="30" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="197"/>
+      <c r="A30" s="199"/>
       <c r="B30" s="113" t="str">
         <f>'Knowledge Base'!$C$25</f>
         <v>Migration Type II</v>
@@ -7964,7 +8093,7 @@
       <c r="BU30" s="83"/>
     </row>
     <row r="31" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="197"/>
+      <c r="A31" s="199"/>
       <c r="B31" s="113" t="str">
         <f>'Knowledge Base'!$C$26</f>
         <v>Migration Type III</v>
@@ -8088,7 +8217,7 @@
       <c r="BU31" s="83"/>
     </row>
     <row r="32" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="198"/>
+      <c r="A32" s="200"/>
       <c r="B32" s="112" t="str">
         <f>'Knowledge Base'!$C$27</f>
         <v>Migration Type IV</v>
@@ -8330,7 +8459,7 @@
       <c r="BU33" s="83"/>
     </row>
     <row r="34" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="197" t="str">
+      <c r="A34" s="199" t="str">
         <f>'Knowledge Base'!$B$28</f>
         <v>Define Scalability Level</v>
       </c>
@@ -8469,7 +8598,7 @@
       <c r="BU34" s="83"/>
     </row>
     <row r="35" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="197"/>
+      <c r="A35" s="199"/>
       <c r="B35" s="113" t="str">
         <f>'Knowledge Base'!$C$29</f>
         <v>OS/VM Level Scaling</v>
@@ -8605,7 +8734,7 @@
       <c r="BU35" s="83"/>
     </row>
     <row r="36" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="197"/>
+      <c r="A36" s="199"/>
       <c r="B36" s="113" t="str">
         <f>'Knowledge Base'!$C$30</f>
         <v>Middleware Level Scaling</v>
@@ -8741,7 +8870,7 @@
       <c r="BU36" s="83"/>
     </row>
     <row r="37" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="197"/>
+      <c r="A37" s="199"/>
       <c r="B37" s="113" t="str">
         <f>'Knowledge Base'!$C$31</f>
         <v>Application Level Scaling</v>
@@ -8881,7 +9010,7 @@
       <c r="BU37" s="83"/>
     </row>
     <row r="38" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="197"/>
+      <c r="A38" s="199"/>
       <c r="B38" s="113" t="str">
         <f>'Knowledge Base'!$C$32</f>
         <v>OS/VM + Middleware Level Scaling</v>
@@ -9017,7 +9146,7 @@
       <c r="BU38" s="83"/>
     </row>
     <row r="39" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="197"/>
+      <c r="A39" s="199"/>
       <c r="B39" s="113" t="str">
         <f>'Knowledge Base'!$C$33</f>
         <v>OS/VM + Application Level Scaling</v>
@@ -9153,7 +9282,7 @@
       <c r="BU39" s="83"/>
     </row>
     <row r="40" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="197"/>
+      <c r="A40" s="199"/>
       <c r="B40" s="113" t="str">
         <f>'Knowledge Base'!$C$34</f>
         <v>Middleware + Application Level Scaling</v>
@@ -9289,7 +9418,7 @@
       <c r="BU40" s="83"/>
     </row>
     <row r="41" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="198"/>
+      <c r="A41" s="200"/>
       <c r="B41" s="112" t="str">
         <f>'Knowledge Base'!$C$35</f>
         <v>OS/VM + Middleware + Application Level Scaling</v>
@@ -9544,7 +9673,7 @@
       <c r="BU42" s="83"/>
     </row>
     <row r="43" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="197" t="str">
+      <c r="A43" s="199" t="str">
         <f>'Knowledge Base'!$B$36</f>
         <v>Select Scaling Type</v>
       </c>
@@ -9643,7 +9772,7 @@
       <c r="BU43" s="83"/>
     </row>
     <row r="44" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="197"/>
+      <c r="A44" s="199"/>
       <c r="B44" s="113" t="str">
         <f>'Knowledge Base'!$C$37</f>
         <v>Horizontal Scaling</v>
@@ -9739,7 +9868,7 @@
       <c r="BU44" s="83"/>
     </row>
     <row r="45" spans="1:73" s="111" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="198"/>
+      <c r="A45" s="200"/>
       <c r="B45" s="112" t="str">
         <f>'Knowledge Base'!$C$38</f>
         <v>Hybrid Scaling</v>
@@ -9955,7 +10084,7 @@
       <c r="BU46" s="83"/>
     </row>
     <row r="47" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="197" t="str">
+      <c r="A47" s="199" t="str">
         <f>'Knowledge Base'!$B$39</f>
         <v>Select Elasticity Automation Degree</v>
       </c>
@@ -10066,7 +10195,7 @@
       <c r="BU47" s="83"/>
     </row>
     <row r="48" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="197"/>
+      <c r="A48" s="199"/>
       <c r="B48" s="113" t="str">
         <f>'Knowledge Base'!$C$40</f>
         <v>Semi-Automatic Scaling</v>
@@ -10173,7 +10302,7 @@
       <c r="BU48" s="83"/>
     </row>
     <row r="49" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="197"/>
+      <c r="A49" s="199"/>
       <c r="B49" s="113" t="str">
         <f>'Knowledge Base'!$C$41</f>
         <v>Semi-Automatic Third-Party Scaling</v>
@@ -10285,7 +10414,7 @@
       <c r="BU49" s="83"/>
     </row>
     <row r="50" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="197"/>
+      <c r="A50" s="199"/>
       <c r="B50" s="113" t="str">
         <f>'Knowledge Base'!$C$42</f>
         <v>Automatic Scaling</v>
@@ -10393,7 +10522,7 @@
       <c r="BU50" s="83"/>
     </row>
     <row r="51" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="198"/>
+      <c r="A51" s="200"/>
       <c r="B51" s="112" t="str">
         <f>'Knowledge Base'!$C$43</f>
         <v>Automatic Third-Party Scaling</v>
@@ -10623,7 +10752,7 @@
       <c r="BU52" s="83"/>
     </row>
     <row r="53" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="197" t="str">
+      <c r="A53" s="199" t="str">
         <f>'Knowledge Base'!$B$44</f>
         <v>Select Scaling Trigger</v>
       </c>
@@ -10734,7 +10863,7 @@
       <c r="BU53" s="83"/>
     </row>
     <row r="54" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="197"/>
+      <c r="A54" s="199"/>
       <c r="B54" s="113" t="str">
         <f>'Knowledge Base'!$C$45</f>
         <v>Event-Driven Trigger</v>
@@ -10846,7 +10975,7 @@
       <c r="BU54" s="83"/>
     </row>
     <row r="55" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="198"/>
+      <c r="A55" s="200"/>
       <c r="B55" s="112" t="str">
         <f>'Knowledge Base'!$C$46</f>
         <v>Proactive Trigger</v>
@@ -11074,7 +11203,7 @@
       <c r="BU56" s="83"/>
     </row>
     <row r="57" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="197" t="str">
+      <c r="A57" s="199" t="str">
         <f>'Knowledge Base'!$B$47</f>
         <v>Select Multi-Tenancy Architecture</v>
       </c>
@@ -11201,7 +11330,7 @@
       <c r="BU57" s="83"/>
     </row>
     <row r="58" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="197"/>
+      <c r="A58" s="199"/>
       <c r="B58" s="113" t="str">
         <f>'Knowledge Base'!$C$48</f>
         <v>Multi-Tenancy Architecture 1</v>
@@ -11323,7 +11452,7 @@
       <c r="BU58" s="83"/>
     </row>
     <row r="59" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="197"/>
+      <c r="A59" s="199"/>
       <c r="B59" s="113" t="str">
         <f>'Knowledge Base'!$C$49</f>
         <v>Multi-Tenancy Architecture 2</v>
@@ -11445,7 +11574,7 @@
       <c r="BU59" s="83"/>
     </row>
     <row r="60" spans="1:73" s="111" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="198"/>
+      <c r="A60" s="200"/>
       <c r="B60" s="112" t="str">
         <f>'Knowledge Base'!$C$50</f>
         <v>Multi-Tenancy Architecture 3</v>
@@ -11687,7 +11816,7 @@
       <c r="BU61" s="83"/>
     </row>
     <row r="62" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="197" t="str">
+      <c r="A62" s="199" t="str">
         <f>'Knowledge Base'!$B$51</f>
         <v>Select Cloud Deployment Model</v>
       </c>
@@ -11786,7 +11915,7 @@
       <c r="BU62" s="83"/>
     </row>
     <row r="63" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="197"/>
+      <c r="A63" s="199"/>
       <c r="B63" s="113" t="str">
         <f>'Knowledge Base'!$C$52</f>
         <v>Private Cloud</v>
@@ -11882,7 +12011,7 @@
       <c r="BU63" s="83"/>
     </row>
     <row r="64" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="197"/>
+      <c r="A64" s="199"/>
       <c r="B64" s="113" t="str">
         <f>'Knowledge Base'!$C$53</f>
         <v>Community Cloud</v>
@@ -11978,7 +12107,7 @@
       <c r="BU64" s="83"/>
     </row>
     <row r="65" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="198"/>
+      <c r="A65" s="200"/>
       <c r="B65" s="112" t="str">
         <f>'Knowledge Base'!$C$54</f>
         <v xml:space="preserve">Hybrid Cloud </v>
@@ -12196,7 +12325,7 @@
       <c r="BU66" s="83"/>
     </row>
     <row r="67" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="197" t="str">
+      <c r="A67" s="199" t="str">
         <f>'Knowledge Base'!$B$55</f>
         <v>Select Cloud Service Model</v>
       </c>
@@ -12335,7 +12464,7 @@
       <c r="BU67" s="83"/>
     </row>
     <row r="68" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="197"/>
+      <c r="A68" s="199"/>
       <c r="B68" s="113" t="str">
         <f>'Knowledge Base'!$C$56</f>
         <v xml:space="preserve">PaaS </v>
@@ -12471,7 +12600,7 @@
       <c r="BU68" s="83"/>
     </row>
     <row r="69" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="197"/>
+      <c r="A69" s="199"/>
       <c r="B69" s="113" t="str">
         <f>'Knowledge Base'!$C$57</f>
         <v>SaaS</v>
@@ -12607,7 +12736,7 @@
       <c r="BU69" s="83"/>
     </row>
     <row r="70" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="197"/>
+      <c r="A70" s="199"/>
       <c r="B70" s="113" t="str">
         <f>'Knowledge Base'!$C$58</f>
         <v>IaaS + PaaS</v>
@@ -12743,7 +12872,7 @@
       <c r="BU70" s="83"/>
     </row>
     <row r="71" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="197"/>
+      <c r="A71" s="199"/>
       <c r="B71" s="113" t="str">
         <f>'Knowledge Base'!$C$59</f>
         <v>IaaS + SaaS</v>
@@ -12879,7 +13008,7 @@
       <c r="BU71" s="83"/>
     </row>
     <row r="72" spans="1:73" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="197"/>
+      <c r="A72" s="199"/>
       <c r="B72" s="113" t="str">
         <f>'Knowledge Base'!$C$60</f>
         <v>PaaS + SaaS</v>
@@ -13015,7 +13144,7 @@
       <c r="BU72" s="83"/>
     </row>
     <row r="73" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="198"/>
+      <c r="A73" s="200"/>
       <c r="B73" s="112" t="str">
         <f>'Knowledge Base'!$C$61</f>
         <v>Iaas + PaaS + SaaS</v>
@@ -13271,7 +13400,7 @@
       <c r="BU74" s="83"/>
     </row>
     <row r="75" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="197" t="str">
+      <c r="A75" s="199" t="str">
         <f>'Knowledge Base'!$B$62</f>
         <v>Define Cloud Hosting</v>
       </c>
@@ -13372,7 +13501,7 @@
       <c r="BU75" s="83"/>
     </row>
     <row r="76" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="197"/>
+      <c r="A76" s="199"/>
       <c r="B76" s="113" t="str">
         <f>'Knowledge Base'!$C$63</f>
         <v>Off-Premise Hosting</v>
@@ -13470,7 +13599,7 @@
       <c r="BU76" s="83"/>
     </row>
     <row r="77" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="198"/>
+      <c r="A77" s="200"/>
       <c r="B77" s="112" t="str">
         <f>'Knowledge Base'!$C$64</f>
         <v>Hybrid Hosting</v>
@@ -13688,7 +13817,7 @@
       <c r="BU78" s="83"/>
     </row>
     <row r="79" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="197" t="str">
+      <c r="A79" s="199" t="str">
         <f>'Knowledge Base'!$B$65</f>
         <v>Define Roles of Responsibility</v>
       </c>
@@ -13787,7 +13916,7 @@
       <c r="BU79" s="83"/>
     </row>
     <row r="80" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="197"/>
+      <c r="A80" s="199"/>
       <c r="B80" s="113" t="str">
         <f>'Knowledge Base'!$C$66</f>
         <v>Role Set 7</v>
@@ -13883,7 +14012,7 @@
       <c r="BU80" s="83"/>
     </row>
     <row r="81" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="197"/>
+      <c r="A81" s="199"/>
       <c r="B81" s="113" t="str">
         <f>'Knowledge Base'!$C$67</f>
         <v>Role Set 8</v>
@@ -13979,7 +14108,7 @@
       <c r="BU81" s="83"/>
     </row>
     <row r="82" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="197"/>
+      <c r="A82" s="199"/>
       <c r="B82" s="113" t="str">
         <f>'Knowledge Base'!$C$68</f>
         <v>Role Set 1 + 7</v>
@@ -14077,7 +14206,7 @@
       <c r="BU82" s="83"/>
     </row>
     <row r="83" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="197"/>
+      <c r="A83" s="199"/>
       <c r="B83" s="113" t="str">
         <f>'Knowledge Base'!$C$69</f>
         <v>Role Set 1 + 8</v>
@@ -14173,7 +14302,7 @@
       <c r="BU83" s="83"/>
     </row>
     <row r="84" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="197"/>
+      <c r="A84" s="199"/>
       <c r="B84" s="113" t="str">
         <f>'Knowledge Base'!$C$70</f>
         <v>Role Set 7 + 8</v>
@@ -14269,7 +14398,7 @@
       <c r="BU84" s="83"/>
     </row>
     <row r="85" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="198"/>
+      <c r="A85" s="200"/>
       <c r="B85" s="112" t="str">
         <f>'Knowledge Base'!$C$71</f>
         <v>Role Set 1 + 7 + 8</v>
@@ -14688,7 +14817,7 @@
       <c r="BU88" s="83"/>
     </row>
     <row r="89" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="197" t="str">
+      <c r="A89" s="199" t="str">
         <f>'Knowledge Base'!$B$73</f>
         <v>Select Pricing Model</v>
       </c>
@@ -14777,7 +14906,7 @@
       <c r="BU89" s="83"/>
     </row>
     <row r="90" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="197"/>
+      <c r="A90" s="199"/>
       <c r="B90" s="113" t="str">
         <f>'Knowledge Base'!$C$74</f>
         <v>Pay-Per-Use</v>
@@ -14863,7 +14992,7 @@
       <c r="BU90" s="83"/>
     </row>
     <row r="91" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="197"/>
+      <c r="A91" s="199"/>
       <c r="B91" s="113" t="str">
         <f>'Knowledge Base'!$C$75</f>
         <v>Pay-Per-Unit</v>
@@ -14949,7 +15078,7 @@
       <c r="BU91" s="83"/>
     </row>
     <row r="92" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="197"/>
+      <c r="A92" s="199"/>
       <c r="B92" s="113" t="str">
         <f>'Knowledge Base'!$C$76</f>
         <v>Charge-Per-Use (Subscription)</v>
@@ -15035,7 +15164,7 @@
       <c r="BU92" s="83"/>
     </row>
     <row r="93" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="198"/>
+      <c r="A93" s="200"/>
       <c r="B93" s="112" t="str">
         <f>'Knowledge Base'!$C$77</f>
         <v>Combined Pricing Model</v>
@@ -15241,7 +15370,7 @@
       <c r="BU94" s="83"/>
     </row>
     <row r="95" spans="1:73" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="197" t="str">
+      <c r="A95" s="199" t="str">
         <f>'Knowledge Base'!$B$78</f>
         <v>Define Resource Location</v>
       </c>
@@ -15336,7 +15465,7 @@
       <c r="BU95" s="83"/>
     </row>
     <row r="96" spans="1:73" s="111" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="198"/>
+      <c r="A96" s="200"/>
       <c r="B96" s="112" t="str">
         <f>'Knowledge Base'!$C$79</f>
         <v>Data Location outside jurisdiction of company</v>
@@ -20055,22 +20184,22 @@
     <mergeCell ref="H2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:BR41 C42:Y42 AA42:BR42 C43:BR47 C48:AW48 AY48:BR48 C49:BR93 C94:AT94 AV94:BC94 BE94:BR94 C95:BR96">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"eb"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="12" operator="beginsWith" text="!">
+    <cfRule type="beginsWith" dxfId="13" priority="12" operator="beginsWith" text="!">
       <formula>LEFT(C3,LEN("!"))="!"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="14" operator="beginsWith" text="?">
+    <cfRule type="beginsWith" dxfId="12" priority="14" operator="beginsWith" text="?">
       <formula>LEFT(C3,LEN("?"))="?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"ex"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>"in"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>"a"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20107,34 +20236,34 @@
     <row r="1" spans="1:18" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="127"/>
       <c r="B1" s="128"/>
-      <c r="C1" s="193" t="str">
+      <c r="C1" s="195" t="str">
         <f>'Knowledge Base'!$A$2</f>
         <v>Distribute Application</v>
       </c>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="195" t="str">
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="196"/>
+      <c r="G1" s="197" t="str">
         <f>'Knowledge Base'!$A$28</f>
         <v>Define Elasticity Strategy</v>
       </c>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="194"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="196"/>
       <c r="K1" s="123" t="str">
         <f>'Knowledge Base'!$A$47</f>
         <v>Define Multi-Tenancy Requirements</v>
       </c>
-      <c r="L1" s="193" t="str">
+      <c r="L1" s="195" t="str">
         <f>'Knowledge Base'!$A$51</f>
         <v>Select Service Provider / Offering</v>
       </c>
-      <c r="M1" s="193"/>
-      <c r="N1" s="193"/>
-      <c r="O1" s="193"/>
-      <c r="P1" s="193"/>
-      <c r="Q1" s="193"/>
-      <c r="R1" s="194"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+      <c r="O1" s="195"/>
+      <c r="P1" s="195"/>
+      <c r="Q1" s="195"/>
+      <c r="R1" s="196"/>
     </row>
     <row r="2" spans="1:18" s="184" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="127"/>
@@ -20207,7 +20336,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="191" t="str">
+      <c r="A3" s="193" t="str">
         <f>'Knowledge Base'!$A$2</f>
         <v>Distribute Application</v>
       </c>
@@ -20235,7 +20364,7 @@
       <c r="R3" s="147"/>
     </row>
     <row r="4" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="191"/>
+      <c r="A4" s="193"/>
       <c r="B4" s="130" t="str">
         <f>'Knowledge Base'!$B$9</f>
         <v>Select Application Tier</v>
@@ -20260,7 +20389,7 @@
       <c r="R4" s="152"/>
     </row>
     <row r="5" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="191"/>
+      <c r="A5" s="193"/>
       <c r="B5" s="130" t="str">
         <f>'Knowledge Base'!$B$16</f>
         <v>Select Application Components</v>
@@ -20287,7 +20416,7 @@
       <c r="R5" s="152"/>
     </row>
     <row r="6" spans="1:18" s="185" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="192"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="131" t="str">
         <f>'Knowledge Base'!$B$24</f>
         <v>Select Migration Type</v>
@@ -20312,7 +20441,7 @@
       <c r="R6" s="157"/>
     </row>
     <row r="7" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="196" t="str">
+      <c r="A7" s="198" t="str">
         <f>'Knowledge Base'!$A$28</f>
         <v>Define Elasticity Strategy</v>
       </c>
@@ -20340,7 +20469,7 @@
       <c r="R7" s="147"/>
     </row>
     <row r="8" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="191"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="175" t="str">
         <f>'Knowledge Base'!$B$36</f>
         <v>Select Scaling Type</v>
@@ -20365,7 +20494,7 @@
       <c r="R8" s="152"/>
     </row>
     <row r="9" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="191"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="175" t="str">
         <f>'Knowledge Base'!$B$39</f>
         <v>Select Elasticity Automation Degree</v>
@@ -20392,7 +20521,7 @@
       <c r="R9" s="152"/>
     </row>
     <row r="10" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="192"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="176" t="str">
         <f>'Knowledge Base'!$B$44</f>
         <v>Select Scaling Trigger</v>
@@ -20445,7 +20574,7 @@
       <c r="R11" s="157"/>
     </row>
     <row r="12" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="191" t="str">
+      <c r="A12" s="193" t="str">
         <f>'Knowledge Base'!$A$51</f>
         <v>Select Service Provider / Offering</v>
       </c>
@@ -20475,7 +20604,7 @@
       <c r="R12" s="147"/>
     </row>
     <row r="13" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="191"/>
+      <c r="A13" s="193"/>
       <c r="B13" s="175" t="str">
         <f>'Knowledge Base'!$B$55</f>
         <v>Select Cloud Service Model</v>
@@ -20498,7 +20627,7 @@
       <c r="R13" s="152"/>
     </row>
     <row r="14" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="191"/>
+      <c r="A14" s="193"/>
       <c r="B14" s="175" t="str">
         <f>'Knowledge Base'!$B$62</f>
         <v>Define Cloud Hosting</v>
@@ -20523,7 +20652,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="191"/>
+      <c r="A15" s="193"/>
       <c r="B15" s="175" t="str">
         <f>'Knowledge Base'!$B$65</f>
         <v>Define Roles of Responsibility</v>
@@ -20550,7 +20679,7 @@
       <c r="R15" s="152"/>
     </row>
     <row r="16" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="191"/>
+      <c r="A16" s="193"/>
       <c r="B16" s="175" t="str">
         <f>'Knowledge Base'!$B$72</f>
         <v>Select Cloud Vendor</v>
@@ -20573,7 +20702,7 @@
       <c r="R16" s="152"/>
     </row>
     <row r="17" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="191"/>
+      <c r="A17" s="193"/>
       <c r="B17" s="175" t="str">
         <f>'Knowledge Base'!$B$73</f>
         <v>Select Pricing Model</v>
@@ -20596,7 +20725,7 @@
       <c r="R17" s="152"/>
     </row>
     <row r="18" spans="1:18" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="192"/>
+      <c r="A18" s="194"/>
       <c r="B18" s="176" t="str">
         <f>'Knowledge Base'!$B$78</f>
         <v>Define Resource Location</v>
@@ -20652,10 +20781,10 @@
     <mergeCell ref="A7:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:R18">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20665,6 +20794,698 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:R14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="222" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="219" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="213" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="223" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="219" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" style="213" customWidth="1"/>
+    <col min="9" max="10" width="12.7109375" style="223" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="219" customWidth="1"/>
+    <col min="12" max="16" width="12.7109375" style="213" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" style="223" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="219"/>
+    <col min="19" max="16384" width="11.42578125" style="213"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="217" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="128"/>
+      <c r="B1" s="195" t="str">
+        <f>'Knowledge Base'!$A$2</f>
+        <v>Distribute Application</v>
+      </c>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="196"/>
+      <c r="F1" s="197" t="str">
+        <f>'Knowledge Base'!$A$28</f>
+        <v>Define Elasticity Strategy</v>
+      </c>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="196"/>
+      <c r="J1" s="123" t="str">
+        <f>'Knowledge Base'!$A$47</f>
+        <v>Define Multi-Tenancy Requirements</v>
+      </c>
+      <c r="K1" s="195" t="str">
+        <f>'Knowledge Base'!$A$51</f>
+        <v>Select Service Provider / Offering</v>
+      </c>
+      <c r="L1" s="195"/>
+      <c r="M1" s="195"/>
+      <c r="N1" s="195"/>
+      <c r="O1" s="195"/>
+      <c r="P1" s="195"/>
+      <c r="Q1" s="196"/>
+      <c r="R1" s="220"/>
+    </row>
+    <row r="2" spans="1:18" s="232" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="186" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="226" t="str">
+        <f>'Knowledge Base'!$B$2</f>
+        <v>Select Application Layer</v>
+      </c>
+      <c r="C2" s="227" t="str">
+        <f>'Knowledge Base'!$B$9</f>
+        <v>Select Application Tier</v>
+      </c>
+      <c r="D2" s="227" t="str">
+        <f>'Knowledge Base'!$B$16</f>
+        <v>Select Application Components</v>
+      </c>
+      <c r="E2" s="228" t="str">
+        <f>'Knowledge Base'!$B$24</f>
+        <v>Select Migration Type</v>
+      </c>
+      <c r="F2" s="229" t="str">
+        <f>'Knowledge Base'!$B$28</f>
+        <v>Define Scalability Level</v>
+      </c>
+      <c r="G2" s="230" t="str">
+        <f>'Knowledge Base'!$B$36</f>
+        <v>Select Scaling Type</v>
+      </c>
+      <c r="H2" s="230" t="str">
+        <f>'Knowledge Base'!$B$39</f>
+        <v>Select Elasticity Automation Degree</v>
+      </c>
+      <c r="I2" s="186" t="str">
+        <f>'Knowledge Base'!$B$44</f>
+        <v>Select Scaling Trigger</v>
+      </c>
+      <c r="J2" s="186" t="str">
+        <f>'Knowledge Base'!$B$47</f>
+        <v>Select Multi-Tenancy Architecture</v>
+      </c>
+      <c r="K2" s="229" t="str">
+        <f>'Knowledge Base'!$B$51</f>
+        <v>Select Cloud Deployment Model</v>
+      </c>
+      <c r="L2" s="230" t="str">
+        <f>'Knowledge Base'!$B$55</f>
+        <v>Select Cloud Service Model</v>
+      </c>
+      <c r="M2" s="230" t="str">
+        <f>'Knowledge Base'!$B$62</f>
+        <v>Define Cloud Hosting</v>
+      </c>
+      <c r="N2" s="230" t="str">
+        <f>'Knowledge Base'!$B$65</f>
+        <v>Define Roles of Responsibility</v>
+      </c>
+      <c r="O2" s="230" t="str">
+        <f>'Knowledge Base'!$B$72</f>
+        <v>Select Cloud Vendor</v>
+      </c>
+      <c r="P2" s="230" t="str">
+        <f>'Knowledge Base'!$B$73</f>
+        <v>Select Pricing Model</v>
+      </c>
+      <c r="Q2" s="186" t="str">
+        <f>'Knowledge Base'!$B$78</f>
+        <v>Define Resource Location</v>
+      </c>
+      <c r="R2" s="231"/>
+    </row>
+    <row r="3" spans="1:18" s="225" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="129" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="148" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="146" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="146" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="147" t="s">
+        <v>187</v>
+      </c>
+      <c r="F3" s="148" t="s">
+        <v>187</v>
+      </c>
+      <c r="G3" s="146" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="146" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" s="147" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="147" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="148" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="147" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="224"/>
+    </row>
+    <row r="4" spans="1:18" s="214" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="130" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="K4" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="L4" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="M4" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="N4" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="R4" s="221"/>
+    </row>
+    <row r="5" spans="1:18" s="214" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="130" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="K5" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="M5" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="N5" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" s="221"/>
+    </row>
+    <row r="6" spans="1:18" s="214" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="130" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="J6" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="L6" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="M6" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="N6" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="151" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q6" s="152" t="s">
+        <v>198</v>
+      </c>
+      <c r="R6" s="221"/>
+    </row>
+    <row r="7" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="188" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="I7" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="160" t="s">
+        <v>187</v>
+      </c>
+      <c r="K7" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="M7" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="N7" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="O7" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="152" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="188" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" s="152" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="L8" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="M8" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="N8" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="O8" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="152" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="188" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" s="152" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="160" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="152" t="s">
+        <v>187</v>
+      </c>
+      <c r="K9" s="149" t="s">
+        <v>187</v>
+      </c>
+      <c r="L9" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="M9" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="N9" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="O9" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="152" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="188" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="215" t="s">
+        <v>198</v>
+      </c>
+      <c r="I10" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="151" t="s">
+        <v>198</v>
+      </c>
+      <c r="O10" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" s="152" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="188" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="218" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="152" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="151" t="s">
+        <v>187</v>
+      </c>
+      <c r="P11" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q11" s="152" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="217" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="189" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="154" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="155" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="155" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="157" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="154" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="155" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="155" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="157" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="157" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="154" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="155" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="155" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="155" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="155" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" s="155" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" s="157" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" s="220"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="216"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:Q1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:Q12">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"Binding"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Affecting"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"Influencing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1">
     <tabColor theme="6" tint="-0.249977111117893"/>
@@ -20701,21 +21522,21 @@
     <row r="1" spans="1:23" s="2" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="57"/>
       <c r="B1" s="55"/>
-      <c r="C1" s="209" t="s">
+      <c r="C1" s="211" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="210"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="212"/>
       <c r="G1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="209" t="s">
+      <c r="H1" s="211" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
-      <c r="K1" s="210"/>
+      <c r="I1" s="209"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="212"/>
       <c r="L1" s="23" t="s">
         <v>44</v>
       </c>
@@ -20725,15 +21546,15 @@
       <c r="N1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="206" t="s">
+      <c r="O1" s="208" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="207"/>
-      <c r="Q1" s="207"/>
-      <c r="R1" s="207"/>
-      <c r="S1" s="207"/>
-      <c r="T1" s="207"/>
-      <c r="U1" s="208"/>
+      <c r="P1" s="209"/>
+      <c r="Q1" s="209"/>
+      <c r="R1" s="209"/>
+      <c r="S1" s="209"/>
+      <c r="T1" s="209"/>
+      <c r="U1" s="210"/>
       <c r="V1" s="23" t="s">
         <v>44</v>
       </c>
@@ -20798,7 +21619,7 @@
       <c r="W2" s="53"/>
     </row>
     <row r="3" spans="1:23" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="206" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="60" t="s">
@@ -20856,7 +21677,7 @@
       <c r="V3" s="26"/>
     </row>
     <row r="4" spans="1:23" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="204"/>
+      <c r="A4" s="206"/>
       <c r="B4" s="61" t="s">
         <v>3</v>
       </c>
@@ -20912,7 +21733,7 @@
       <c r="V4" s="26"/>
     </row>
     <row r="5" spans="1:23" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="204"/>
+      <c r="A5" s="206"/>
       <c r="B5" s="60" t="s">
         <v>4</v>
       </c>
@@ -20968,7 +21789,7 @@
       <c r="V5" s="26"/>
     </row>
     <row r="6" spans="1:23" s="9" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="205"/>
+      <c r="A6" s="207"/>
       <c r="B6" s="62" t="s">
         <v>5</v>
       </c>
@@ -21024,7 +21845,7 @@
       <c r="V6" s="27"/>
     </row>
     <row r="7" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="200" t="s">
+      <c r="A7" s="202" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="17" t="s">
@@ -21082,7 +21903,7 @@
       <c r="V7" s="26"/>
     </row>
     <row r="8" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="191"/>
+      <c r="A8" s="193"/>
       <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
@@ -21138,7 +21959,7 @@
       <c r="V8" s="26"/>
     </row>
     <row r="9" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="191"/>
+      <c r="A9" s="193"/>
       <c r="B9" s="17" t="s">
         <v>12</v>
       </c>
@@ -21194,7 +22015,7 @@
       <c r="V9" s="26"/>
     </row>
     <row r="10" spans="1:23" s="10" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="192"/>
+      <c r="A10" s="194"/>
       <c r="B10" s="93" t="s">
         <v>13</v>
       </c>
@@ -21308,7 +22129,7 @@
       <c r="V11" s="74"/>
     </row>
     <row r="12" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="200" t="s">
+      <c r="A12" s="202" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -21366,7 +22187,7 @@
       <c r="V12" s="26"/>
     </row>
     <row r="13" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="201"/>
+      <c r="A13" s="203"/>
       <c r="B13" s="17" t="s">
         <v>32</v>
       </c>
@@ -21422,7 +22243,7 @@
       <c r="V13" s="26"/>
     </row>
     <row r="14" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="201"/>
+      <c r="A14" s="203"/>
       <c r="B14" s="17" t="s">
         <v>34</v>
       </c>
@@ -21478,7 +22299,7 @@
       <c r="V14" s="26"/>
     </row>
     <row r="15" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="201"/>
+      <c r="A15" s="203"/>
       <c r="B15" s="17" t="s">
         <v>35</v>
       </c>
@@ -21534,7 +22355,7 @@
       <c r="V15" s="26"/>
     </row>
     <row r="16" spans="1:23" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="201"/>
+      <c r="A16" s="203"/>
       <c r="B16" s="91" t="s">
         <v>38</v>
       </c>
@@ -21590,7 +22411,7 @@
       <c r="V16" s="26"/>
     </row>
     <row r="17" spans="1:22" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="202"/>
+      <c r="A17" s="204"/>
       <c r="B17" s="92" t="s">
         <v>31</v>
       </c>
@@ -21646,7 +22467,7 @@
       <c r="V17" s="22"/>
     </row>
     <row r="18" spans="1:22" s="10" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="203"/>
+      <c r="A18" s="205"/>
       <c r="B18" s="93" t="s">
         <v>39</v>
       </c>

</xml_diff>